<commit_message>
Updated time log and uncommented except
</commit_message>
<xml_diff>
--- a/Python RSI Scraper/Time log.xlsx
+++ b/Python RSI Scraper/Time log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acure\Desktop\Stock Scraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acure\Documents\GitHub\JacobJohnsonProjects\Python RSI Scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3ECE14-BC8A-49AF-A16B-FF1519C56E65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DCAC26-C248-4217-9102-8C2CDA942BBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{080D563C-2D4C-40B5-8C20-7231652D5B0B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date:</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Created RSI calculation function</t>
+  </si>
+  <si>
+    <t>Created web scraper and did some admin work for github</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +461,7 @@
     <col min="1" max="1" width="17.33203125" style="8" customWidth="1"/>
     <col min="2" max="3" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,7 +504,7 @@
       </c>
       <c r="F2" s="3">
         <f>SUM(D2:D1000)</f>
-        <v>5.208333333333337E-2</v>
+        <v>0.11249999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -515,7 +518,7 @@
         <v>0.39305555555555555</v>
       </c>
       <c r="D3" s="3">
-        <f>IFERROR(IF(C3-B3&lt;&gt;0, C3-B3,""),"")</f>
+        <f>IF(C3-B3&lt;&gt;0, C3-B3,"")</f>
         <v>3.4027777777777768E-2</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -523,14 +526,26 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="3" t="str">
-        <f t="shared" ref="D3:D24" si="0">IF(C4-B4&lt;&gt;0, C4-B4,"")</f>
-        <v/>
+      <c r="A4" s="9">
+        <v>44325</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="D4" s="3">
+        <f>IF(C4-B4&lt;&gt;0, C4-B4,"")</f>
+        <v>6.0416666666666619E-2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:D24" si="0">IF(C5-B5&lt;&gt;0, C5-B5,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>